<commit_message>
automatisation profs dans chaque ressource
</commit_message>
<xml_diff>
--- a/Documents/QuiFaitQuoiPOURTEST.xlsx
+++ b/Documents/QuiFaitQuoiPOURTEST.xlsx
@@ -823,7 +823,7 @@
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.63"/>
@@ -1874,7 +1874,7 @@
       <selection pane="topLeft" activeCell="K41" activeCellId="0" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.63"/>
@@ -2293,10 +2293,10 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>